<commit_message>
adjusted for optimal settings NN in sim 2 10
</commit_message>
<xml_diff>
--- a/efficiency_testing/sim_2_10/Optimizer_Testing_NN_propensity.xlsx
+++ b/efficiency_testing/sim_2_10/Optimizer_Testing_NN_propensity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcg\Google Drive\MasterThesis\dml_est_general\efficiency_testing\sim_2_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7D701B-2103-4804-8121-695E10530A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC25E81-3F25-4BAA-9AEF-947C2AB3F262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3444" yWindow="1104" windowWidth="17448" windowHeight="10320" activeTab="1" xr2:uid="{6A5FBCD0-C166-4D81-9F0C-49E81C69DCD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6A5FBCD0-C166-4D81-9F0C-49E81C69DCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Single_Layer" sheetId="4" r:id="rId1"/>
@@ -163,12 +163,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -235,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -251,6 +257,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0013E5D1-B0BE-4F3F-93C2-18356612F2E4}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,22 +767,54 @@
       <c r="B7" s="1">
         <v>0.01</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
+      <c r="C7" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4.42</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4.16</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3.59</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="K7" s="1">
+        <v>6.44</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5.21</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="O7" s="1">
+        <v>5.21</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -784,22 +823,54 @@
       <c r="B8" s="1">
         <v>0.01</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="C8" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4.09</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3.76</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="K8" s="1">
+        <v>7.57</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="M8" s="1">
+        <v>8.16</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="O8" s="1">
+        <v>5.97</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>5.42</v>
+      </c>
+      <c r="R8" s="7">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -808,22 +879,54 @@
       <c r="B9" s="1">
         <v>0.1</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="C9" s="1">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3.71</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3.67</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="K9" s="1">
+        <v>8.65</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="M9" s="1">
+        <v>8</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="O9" s="1">
+        <v>6.56</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>6.37</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -832,22 +935,54 @@
       <c r="B10" s="1">
         <v>0.01</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="C10" s="1">
+        <v>3.88</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3.59</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3.31</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="K10" s="1">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="M10" s="1">
+        <v>4.03</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="O10" s="1">
+        <v>3.83</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -856,22 +991,54 @@
       <c r="B11" s="1">
         <v>0.01</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="C11" s="1">
+        <v>34.74</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="E11" s="1">
+        <v>33.96</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="G11" s="1">
+        <v>29.57</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="I11" s="1">
+        <v>27.47</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="K11" s="1">
+        <v>36.07</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="M11" s="1">
+        <v>35.29</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="O11" s="1">
+        <v>33.9</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>35.4</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -879,35 +1046,35 @@
       </c>
       <c r="D13">
         <f>MIN(D7:D11)</f>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="F13">
         <f t="shared" ref="F13:R13" si="0">MIN(F7:F11)</f>
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="P13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -916,7 +1083,7 @@
       </c>
       <c r="D14">
         <f>MIN(D13:R13)</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -939,21 +1106,21 @@
         <f>IF(_xlfn.MINIFS(I7:I11,J7:J11,$D$14) = 0, NA(), _xlfn.MINIFS(I7:I11,J7:J11,$D$14))</f>
         <v>#N/A</v>
       </c>
-      <c r="L15" t="e">
+      <c r="L15">
         <f>IF(_xlfn.MINIFS(K7:K11,L7:L11,$D$14) = 0, NA(), _xlfn.MINIFS(K7:K11,L7:L11,$D$14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N15" t="e">
+        <v>7.57</v>
+      </c>
+      <c r="N15">
         <f>IF(_xlfn.MINIFS(M7:M11,N7:N11,$D$14) = 0, NA(), _xlfn.MINIFS(M7:M11,N7:N11,$D$14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P15" t="e">
+        <v>8</v>
+      </c>
+      <c r="P15">
         <f>IF(_xlfn.MINIFS(O7:O11,P7:P11,$D$14) = 0, NA(), _xlfn.MINIFS(O7:O11,P7:P11,$D$14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R15" t="e">
+        <v>6.56</v>
+      </c>
+      <c r="R15">
         <f>IF(_xlfn.MINIFS(Q7:Q11,R7:R11,$D$14) = 0, NA(), _xlfn.MINIFS(Q7:Q11,R7:R11,$D$14))</f>
-        <v>#N/A</v>
+        <v>5.42</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -962,22 +1129,11 @@
       </c>
       <c r="D16" cm="1">
         <f t="array" ref="D16">MIN(IF(ISNUMBER(D15:R15),D15:R15,""))</f>
-        <v>0</v>
+        <v>5.42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="Q5:R5"/>
@@ -994,6 +1150,17 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1004,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166A5B32-9AC9-417B-B8AA-7D7202DC2B5D}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:R26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,22 +1364,54 @@
       <c r="B7" s="1">
         <v>0.01</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
+      <c r="C7" s="1">
+        <v>3.77</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3.49</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3.84</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3.44</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="K7" s="1">
+        <v>4.41</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="M7" s="1">
+        <v>4.28</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="O7" s="1">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1221,22 +1420,54 @@
       <c r="B8" s="1">
         <v>0.01</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="C8" s="1">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4.74</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="I8" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="K8" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="O8" s="1">
+        <v>5.39</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>4.82</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1245,22 +1476,54 @@
       <c r="B9" s="1">
         <v>0.1</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="C9" s="1">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3.96</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3.96</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="K9" s="1">
+        <v>6.39</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="M9" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="O9" s="1">
+        <v>6.42</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>6.36</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1269,22 +1532,54 @@
       <c r="B10" s="1">
         <v>0.01</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="C10" s="1">
+        <v>3.93</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3.55</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3.85</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3.54</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="K10" s="1">
+        <v>4.13</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="M10" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="O10" s="1">
+        <v>4.49</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>3.89</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1293,22 +1588,54 @@
       <c r="B11" s="1">
         <v>0.01</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="C11" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="E11" s="1">
+        <v>26.59</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="G11" s="1">
+        <v>28.65</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="I11" s="1">
+        <v>25.24</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="K11" s="1">
+        <v>30.57</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="M11" s="1">
+        <v>30.18</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="O11" s="1">
+        <v>30.2</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>29.73</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1316,35 +1643,35 @@
       </c>
       <c r="D13">
         <f>MIN(D7:D11)</f>
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="F13">
         <f t="shared" ref="F13:R13" si="0">MIN(F7:F11)</f>
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="P13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -1353,7 +1680,7 @@
       </c>
       <c r="D14">
         <f>MIN(D13:R13)</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -1388,9 +1715,9 @@
         <f>IF(_xlfn.MINIFS(O7:O11,P7:P11,$D$14) = 0, NA(), _xlfn.MINIFS(O7:O11,P7:P11,$D$14))</f>
         <v>#N/A</v>
       </c>
-      <c r="R15" t="e">
+      <c r="R15">
         <f>IF(_xlfn.MINIFS(Q7:Q11,R7:R11,$D$14) = 0, NA(), _xlfn.MINIFS(Q7:Q11,R7:R11,$D$14))</f>
-        <v>#N/A</v>
+        <v>29.73</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1399,7 +1726,7 @@
       </c>
       <c r="D16" cm="1">
         <f t="array" ref="D16">MIN(IF(ISNUMBER(D15:R15),D15:R15,""))</f>
-        <v>0</v>
+        <v>29.73</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
@@ -1582,22 +1909,54 @@
       <c r="B22" s="1">
         <v>0.01</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
+      <c r="C22" s="1">
+        <v>4.43</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E22" s="1">
+        <v>4.46</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="G22" s="1">
+        <v>4.34</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="I22" s="1">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="K22" s="1">
+        <v>6.16</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="M22" s="1">
+        <v>5.16</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="O22" s="1">
+        <v>5.29</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>4.97</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -1606,22 +1965,54 @@
       <c r="B23" s="1">
         <v>0.01</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
+      <c r="C23" s="1">
+        <v>6.71</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="E23" s="1">
+        <v>6.38</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="G23" s="1">
+        <v>5.38</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="I23" s="1">
+        <v>5.85</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="K23" s="1">
+        <v>8.31</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="M23" s="1">
+        <v>7.72</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="O23" s="1">
+        <v>9.09</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>7.23</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -1630,22 +2021,54 @@
       <c r="B24" s="1">
         <v>0.1</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
+      <c r="C24" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="E24" s="1">
+        <v>6.35</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="G24" s="1">
+        <v>6.56</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="I24" s="1">
+        <v>6.24</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="K24" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="M24" s="1">
+        <v>14.18</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="O24" s="1">
+        <v>13.64</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>11.64</v>
+      </c>
+      <c r="R24" s="1">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -1654,22 +2077,54 @@
       <c r="B25" s="1">
         <v>0.01</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
+      <c r="C25" s="1">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3.78</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="G25" s="1">
+        <v>4.07</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="I25" s="1">
+        <v>3.61</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="K25" s="1">
+        <v>5.01</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="M25" s="1">
+        <v>4.24</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="O25" s="1">
+        <v>4.53</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>4.29</v>
+      </c>
+      <c r="R25" s="1">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -1678,22 +2133,54 @@
       <c r="B26" s="1">
         <v>0.01</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+      <c r="C26" s="1">
+        <v>29.67</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="E26" s="1">
+        <v>29.8</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="G26" s="1">
+        <v>25.15</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="I26" s="1">
+        <v>29.95</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="K26" s="1">
+        <v>8.65</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="M26" s="1">
+        <v>8.66</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="O26" s="1">
+        <v>6.37</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>6.68</v>
+      </c>
+      <c r="R26" s="1">
+        <v>0.37</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -1701,35 +2188,35 @@
       </c>
       <c r="D28">
         <f>MIN(D22:D26)</f>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="F28">
         <f t="shared" ref="F28" si="1">MIN(F22:F26)</f>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="H28">
         <f t="shared" ref="H28" si="2">MIN(H22:H26)</f>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="J28">
         <f t="shared" ref="J28" si="3">MIN(J22:J26)</f>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="L28">
         <f t="shared" ref="L28" si="4">MIN(L22:L26)</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="N28">
         <f t="shared" ref="N28" si="5">MIN(N22:N26)</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="P28">
         <f t="shared" ref="P28" si="6">MIN(P22:P26)</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="R28">
         <f t="shared" ref="R28" si="7">MIN(R22:R26)</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -1738,7 +2225,7 @@
       </c>
       <c r="D29">
         <f>MIN(D28:R28)</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -1746,36 +2233,36 @@
         <v>24</v>
       </c>
       <c r="D30" t="e">
-        <f>IF(_xlfn.MINIFS(C22:C26,D22:D26,$D$14) = 0, NA(), _xlfn.MINIFS(C22:C26,D22:D26,$D$14))</f>
+        <f>IF(_xlfn.MINIFS(C22:C26,D22:D26,$D$29) = 0, NA(), _xlfn.MINIFS(C22:C26,D22:D26,$D$29))</f>
         <v>#N/A</v>
       </c>
       <c r="F30" t="e">
-        <f>IF(_xlfn.MINIFS(E22:E26,F22:F26,$D$14) = 0, NA(), _xlfn.MINIFS(E22:E26,F22:F26,$D$14))</f>
+        <f>IF(_xlfn.MINIFS(E22:E26,F22:F26,$D$29) = 0, NA(), _xlfn.MINIFS(E22:E26,F22:F26,$D$29))</f>
         <v>#N/A</v>
       </c>
       <c r="H30" t="e">
-        <f>IF(_xlfn.MINIFS(G22:G26,H22:H26,$D$14) = 0, NA(), _xlfn.MINIFS(G22:G26,H22:H26,$D$14))</f>
+        <f>IF(_xlfn.MINIFS(G22:G26,H22:H26,$D$29) = 0, NA(), _xlfn.MINIFS(G22:G26,H22:H26,$D$29))</f>
         <v>#N/A</v>
       </c>
       <c r="J30" t="e">
-        <f>IF(_xlfn.MINIFS(I22:I26,J22:J26,$D$14) = 0, NA(), _xlfn.MINIFS(I22:I26,J22:J26,$D$14))</f>
+        <f>IF(_xlfn.MINIFS(I22:I26,J22:J26,$D$29) = 0, NA(), _xlfn.MINIFS(I22:I26,J22:J26,$D$29))</f>
         <v>#N/A</v>
       </c>
-      <c r="L30" t="e">
-        <f>IF(_xlfn.MINIFS(K22:K26,L22:L26,$D$14) = 0, NA(), _xlfn.MINIFS(K22:K26,L22:L26,$D$14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N30" t="e">
-        <f>IF(_xlfn.MINIFS(M22:M26,N22:N26,$D$14) = 0, NA(), _xlfn.MINIFS(M22:M26,N22:N26,$D$14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P30" t="e">
-        <f>IF(_xlfn.MINIFS(O22:O26,P22:P26,$D$14) = 0, NA(), _xlfn.MINIFS(O22:O26,P22:P26,$D$14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R30" t="e">
-        <f>IF(_xlfn.MINIFS(Q22:Q26,R22:R26,$D$14) = 0, NA(), _xlfn.MINIFS(Q22:Q26,R22:R26,$D$14))</f>
-        <v>#N/A</v>
+      <c r="L30">
+        <f>IF(_xlfn.MINIFS(K22:K26,L22:L26,$D$29) = 0, NA(), _xlfn.MINIFS(K22:K26,L22:L26,$D$29))</f>
+        <v>8.31</v>
+      </c>
+      <c r="N30">
+        <f>IF(_xlfn.MINIFS(M22:M26,N22:N26,$D$29) = 0, NA(), _xlfn.MINIFS(M22:M26,N22:N26,$D$29))</f>
+        <v>7.72</v>
+      </c>
+      <c r="P30">
+        <f>IF(_xlfn.MINIFS(O22:O26,P22:P26,$D$29) = 0, NA(), _xlfn.MINIFS(O22:O26,P22:P26,$D$29))</f>
+        <v>13.64</v>
+      </c>
+      <c r="R30">
+        <f>IF(_xlfn.MINIFS(Q22:Q26,R22:R26,$D$29) = 0, NA(), _xlfn.MINIFS(Q22:Q26,R22:R26,$D$29))</f>
+        <v>7.23</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -1784,49 +2271,11 @@
       </c>
       <c r="D31">
         <f t="array" ref="D31">MIN(IF(ISNUMBER(D30:R30),D30:R30,""))</f>
-        <v>0</v>
+        <v>7.23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
@@ -1843,6 +2292,44 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>